<commit_message>
Updates 12s, 16s code to include a ADFG mapped taxa list; works toward geographically accurate mapped unresolved taxa lists for ADFG
</commit_message>
<xml_diff>
--- a/Deliverables/12S/WADE003-arcticpred-12SP1-taxa-output_unresolved.xlsx
+++ b/Deliverables/12S/WADE003-arcticpred-12SP1-taxa-output_unresolved.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5bd2331949789710/文档/WADE LAB/Arctic-predator-diet-microbiome/Deliverables/12S/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MBall\OneDrive\Documents\UW-DOCS\WADE lab\Arctic-predator-diet-microbiome\Deliverables\12S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C90B1C4A-C584-4C48-BA42-7B2FF5DA1812}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F72B78-5113-47FB-915A-345CC5B4B5DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D5BE2BDA-A88E-4643-9D78-B50402266002}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" xr2:uid="{D5BE2BDA-A88E-4643-9D78-B50402266002}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -722,7 +722,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -737,6 +737,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -754,7 +760,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -765,6 +771,9 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1103,16 +1112,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A0E6851-D96E-47FD-8F8E-1962ADAEEF69}">
   <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="22.265625" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="9" max="10" width="255.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="61.86328125" customWidth="1"/>
+    <col min="10" max="10" width="255.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1144,143 +1154,143 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="J2" s="7"/>
+    </row>
+    <row r="3" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="J3" s="7"/>
+    </row>
+    <row r="4" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="J4" s="7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="I5" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="I6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="J6" s="7"/>
+    </row>
+    <row r="7" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="B7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="I7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="7"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>34</v>
       </c>
@@ -1304,7 +1314,7 @@
       </c>
       <c r="J8" s="3"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>38</v>
       </c>
@@ -1328,7 +1338,7 @@
       </c>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>39</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>42</v>
       </c>
@@ -1384,7 +1394,7 @@
       </c>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -1410,7 +1420,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>48</v>
       </c>
@@ -1440,7 +1450,7 @@
       </c>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>53</v>
       </c>
@@ -1464,7 +1474,7 @@
       </c>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1488,7 +1498,7 @@
       </c>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -1514,7 +1524,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -1540,7 +1550,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1566,7 +1576,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
         <v>63</v>
       </c>
@@ -1595,7 +1605,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
         <v>66</v>
       </c>
@@ -1624,7 +1634,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>68</v>
       </c>
@@ -1648,7 +1658,7 @@
       </c>
       <c r="J21" s="3"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>69</v>
       </c>
@@ -1674,7 +1684,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>72</v>
       </c>
@@ -1701,7 +1711,7 @@
       </c>
       <c r="J23" s="3"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>74</v>
       </c>
@@ -1728,7 +1738,7 @@
       </c>
       <c r="J24" s="3"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>77</v>
       </c>
@@ -1752,7 +1762,7 @@
       </c>
       <c r="J25" s="3"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>79</v>
       </c>
@@ -1782,7 +1792,7 @@
       </c>
       <c r="J26" s="3"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
         <v>80</v>
       </c>
@@ -1806,7 +1816,7 @@
       </c>
       <c r="J27" s="3"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>82</v>
       </c>
@@ -1832,7 +1842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
         <v>83</v>
       </c>
@@ -1858,7 +1868,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -1884,7 +1894,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>85</v>
       </c>
@@ -1907,7 +1917,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>88</v>
       </c>
@@ -1934,7 +1944,7 @@
       </c>
       <c r="J32" s="3"/>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>90</v>
       </c>
@@ -1958,7 +1968,7 @@
       </c>
       <c r="J33" s="3"/>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
         <v>92</v>
       </c>
@@ -1984,7 +1994,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
         <v>95</v>
       </c>
@@ -2010,7 +2020,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -2036,7 +2046,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -2057,7 +2067,7 @@
       </c>
       <c r="J37" s="3"/>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
         <v>100</v>
       </c>
@@ -2081,7 +2091,7 @@
       </c>
       <c r="J38" s="3"/>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
         <v>101</v>
       </c>
@@ -2110,7 +2120,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
         <v>107</v>
       </c>
@@ -2136,7 +2146,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
         <v>110</v>
       </c>
@@ -2162,7 +2172,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
         <v>111</v>
       </c>
@@ -2188,7 +2198,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
         <v>112</v>
       </c>
@@ -2214,7 +2224,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
         <v>113</v>
       </c>
@@ -2238,7 +2248,7 @@
       </c>
       <c r="J44" s="3"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
         <v>114</v>
       </c>
@@ -2262,7 +2272,7 @@
       </c>
       <c r="J45" s="3"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
         <v>116</v>
       </c>
@@ -2288,7 +2298,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
         <v>117</v>
       </c>
@@ -2314,7 +2324,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
         <v>118</v>
       </c>
@@ -2340,7 +2350,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
         <v>121</v>
       </c>
@@ -2366,7 +2376,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
         <v>122</v>
       </c>
@@ -2392,7 +2402,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
         <v>123</v>
       </c>
@@ -2418,7 +2428,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A52" t="s">
         <v>124</v>
       </c>
@@ -2447,7 +2457,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A53" t="s">
         <v>125</v>
       </c>
@@ -2473,7 +2483,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
         <v>126</v>
       </c>
@@ -2497,7 +2507,7 @@
       </c>
       <c r="J54" s="3"/>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
         <v>128</v>
       </c>
@@ -2523,7 +2533,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
         <v>131</v>
       </c>
@@ -2550,7 +2560,7 @@
       </c>
       <c r="J56" s="3"/>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A57" t="s">
         <v>134</v>
       </c>
@@ -2579,7 +2589,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A58" t="s">
         <v>137</v>
       </c>
@@ -2608,7 +2618,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A59" t="s">
         <v>138</v>
       </c>
@@ -2634,7 +2644,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
         <v>139</v>
       </c>
@@ -2658,7 +2668,7 @@
       </c>
       <c r="J60" s="3"/>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
         <v>141</v>
       </c>
@@ -2690,7 +2700,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
         <v>143</v>
       </c>
@@ -2719,7 +2729,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A63" t="s">
         <v>144</v>
       </c>
@@ -2743,7 +2753,7 @@
       </c>
       <c r="J63" s="3"/>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -2767,7 +2777,7 @@
       </c>
       <c r="J64" s="3"/>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A65" t="s">
         <v>148</v>
       </c>
@@ -2778,7 +2788,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>151</v>
       </c>
@@ -2802,7 +2812,7 @@
       </c>
       <c r="J66" s="3"/>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
         <v>153</v>
       </c>
@@ -2826,7 +2836,7 @@
       </c>
       <c r="J67" s="3"/>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A68" t="s">
         <v>154</v>
       </c>
@@ -2853,7 +2863,7 @@
       </c>
       <c r="J68" s="3"/>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A69" t="s">
         <v>156</v>
       </c>
@@ -2864,7 +2874,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A70" t="s">
         <v>159</v>
       </c>
@@ -2888,7 +2898,7 @@
       </c>
       <c r="J70" s="3"/>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A71" t="s">
         <v>161</v>
       </c>
@@ -2912,7 +2922,7 @@
       </c>
       <c r="J71" s="3"/>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A72" t="s">
         <v>162</v>
       </c>
@@ -2932,7 +2942,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A73" t="s">
         <v>163</v>
       </c>
@@ -2956,7 +2966,7 @@
       </c>
       <c r="J73" s="3"/>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A74" t="s">
         <v>164</v>
       </c>
@@ -2986,7 +2996,7 @@
       </c>
       <c r="J74" s="3"/>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A75" t="s">
         <v>167</v>
       </c>
@@ -3015,7 +3025,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A76" t="s">
         <v>171</v>
       </c>
@@ -3039,7 +3049,7 @@
       </c>
       <c r="J76" s="3"/>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A77" t="s">
         <v>172</v>
       </c>
@@ -3071,7 +3081,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A78" t="s">
         <v>175</v>
       </c>
@@ -3101,7 +3111,7 @@
       </c>
       <c r="J78" s="3"/>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A79" t="s">
         <v>177</v>
       </c>
@@ -3133,7 +3143,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A80" t="s">
         <v>179</v>
       </c>
@@ -3165,7 +3175,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A81" t="s">
         <v>186</v>
       </c>
@@ -3191,7 +3201,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A82" t="s">
         <v>187</v>
       </c>
@@ -3223,7 +3233,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A83" t="s">
         <v>188</v>
       </c>
@@ -3252,7 +3262,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A84" t="s">
         <v>194</v>
       </c>
@@ -3284,7 +3294,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A85" t="s">
         <v>201</v>
       </c>
@@ -3310,16 +3320,16 @@
         <v>203</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:10" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A86" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="I86" s="3" t="s">
+      <c r="I86" s="7" t="s">
         <v>205</v>
       </c>
-      <c r="J86" s="3"/>
-    </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J86" s="7"/>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A87" t="s">
         <v>206</v>
       </c>
@@ -3343,7 +3353,7 @@
       </c>
       <c r="J87" s="3"/>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A88" t="s">
         <v>207</v>
       </c>
@@ -3370,7 +3380,7 @@
       </c>
       <c r="J88" s="3"/>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A89" t="s">
         <v>211</v>
       </c>
@@ -3396,15 +3406,15 @@
         <v>203</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.45">
       <c r="I90" s="3"/>
       <c r="J90" s="3"/>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.45">
       <c r="I91" s="3"/>
       <c r="J91" s="3"/>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.45">
       <c r="I92" s="3"/>
       <c r="J92" s="3"/>
     </row>

</xml_diff>